<commit_message>
Mise a jour majeure avant l'envoi du premier livrable
</commit_message>
<xml_diff>
--- a/doc/Gestion des coûts/Gestion des coûts Projet S3.xlsx
+++ b/doc/Gestion des coûts/Gestion des coûts Projet S3.xlsx
@@ -26,12 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
-    <t xml:space="preserve">Département info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projets tutorés 2016-17</t>
+    <t xml:space="preserve">P7 – Client SNMP Android</t>
   </si>
   <si>
     <t xml:space="preserve">Coût estimé du projet</t>
@@ -88,13 +85,16 @@
     <t xml:space="preserve">IUT Valence</t>
   </si>
   <si>
+    <t xml:space="preserve">Projets tutorés 2016-17</t>
+  </si>
+  <si>
     <t xml:space="preserve">mis à jour le: </t>
   </si>
   <si>
     <t xml:space="preserve">Version 1.6</t>
   </si>
   <si>
-    <t xml:space="preserve">P7 – Client SNMP Android</t>
+    <t xml:space="preserve">Département informatique</t>
   </si>
   <si>
     <t xml:space="preserve">Coût actuel du projet</t>
@@ -413,16 +413,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -505,10 +509,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -523,6 +523,10 @@
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -611,10 +615,6 @@
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -727,7 +727,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Evolution du coût de revient'!$B$7</c:f>
+              <c:f>'Evolution du coût de revient'!$C$7:$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -767,7 +767,7 @@
           </c:dLbls>
           <c:yVal>
             <c:numRef>
-              <c:f>'Evolution du coût de revient'!$C$7:$Q$7</c:f>
+              <c:f>'Evolution du coût de revient'!$D$7:$R$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -821,11 +821,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="29956695"/>
-        <c:axId val="84414880"/>
+        <c:axId val="18242793"/>
+        <c:axId val="1277854"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29956695"/>
+        <c:axId val="18242793"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -862,14 +862,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84414880"/>
+        <c:crossAx val="1277854"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84414880"/>
+        <c:axId val="1277854"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +913,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29956695"/>
+        <c:crossAx val="18242793"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -954,16 +954,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1163160</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>810720</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>832320</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>478800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -976,8 +976,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17907840" y="0"/>
-          <a:ext cx="1117080" cy="648000"/>
+          <a:off x="18212760" y="0"/>
+          <a:ext cx="1125360" cy="646920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>868680</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1176120</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1220760" y="0"/>
+          <a:ext cx="1526760" cy="605520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -997,19 +1034,19 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>33120</xdr:colOff>
+      <xdr:colOff>2290320</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1121400</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>767880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 1" descr=""/>
+        <xdr:cNvPr id="2" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1018,8 +1055,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19368720" y="360"/>
-          <a:ext cx="1088280" cy="648000"/>
+          <a:off x="19692360" y="360"/>
+          <a:ext cx="1125360" cy="646920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>868320</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1175760</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1220400" y="0"/>
+          <a:ext cx="1526760" cy="605520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1038,20 +1112,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>481320</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>128880</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>368280</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>272160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr=""/>
+        <xdr:cNvPr id="4" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1060,8 +1134,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13140000" y="19440"/>
-          <a:ext cx="1086840" cy="648000"/>
+          <a:off x="13273200" y="19440"/>
+          <a:ext cx="1086120" cy="646920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1075,25 +1149,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>49320</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>5040</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvPr id="5" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="992160" y="1664280"/>
-        <a:ext cx="14672880" cy="3232800"/>
+        <a:off x="1344600" y="1634040"/>
+        <a:ext cx="14547960" cy="2988000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1105,26 +1179,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>709920</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>357480</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>513000</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Line 1"/>
+        <xdr:cNvPr id="6" name="Line 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1652760" y="2214000"/>
-          <a:ext cx="12119040" cy="0"/>
+          <a:ext cx="12252240" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1148,6 +1222,43 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>593280</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1176840</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="945360" y="0"/>
+          <a:ext cx="1526760" cy="605520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1155,20 +1266,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>464040</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>111600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>739800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>43560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 1" descr=""/>
+        <xdr:cNvPr id="8" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1177,8 +1288,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13389120" y="19800"/>
-          <a:ext cx="1085400" cy="648000"/>
+          <a:off x="13475160" y="19800"/>
+          <a:ext cx="1084320" cy="646920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>240840</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>79920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1618920" y="0"/>
+          <a:ext cx="1526760" cy="605520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1206,34 +1354,32 @@
   </sheetPr>
   <dimension ref="1:33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="1" sqref="H20 H33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="1" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="2" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.96356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="2" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="2" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="2" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="0"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
       <c r="K1" s="0"/>
@@ -2253,10 +2399,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="3"/>
+      <c r="B2" s="0"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="0"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -3279,10 +3425,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="0"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="0"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
@@ -4304,22 +4450,22 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="0"/>
+      <c r="A5" s="0"/>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
       <c r="O5" s="0"/>
       <c r="P5" s="0"/>
       <c r="Q5" s="0"/>
@@ -5332,20 +5478,20 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="0"/>
+      <c r="A6" s="0"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
       <c r="O6" s="0"/>
       <c r="P6" s="0"/>
       <c r="Q6" s="0"/>
@@ -6358,38 +6504,38 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="0"/>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
+      <c r="J7" s="6"/>
+      <c r="K7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
+      <c r="L7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="M7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="N7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="0"/>
       <c r="O7" s="0"/>
       <c r="P7" s="0"/>
       <c r="Q7" s="0"/>
@@ -7402,36 +7548,36 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="0"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="0"/>
+      <c r="N8" s="8"/>
       <c r="O8" s="0"/>
       <c r="P8" s="0"/>
       <c r="Q8" s="0"/>
@@ -8444,48 +8590,48 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="0"/>
+      <c r="B9" s="11" t="n">
         <v>42639</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="C9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="12" t="n">
+      <c r="D9" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="11" t="n">
+      <c r="E9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="12" t="n">
+      <c r="F9" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="11" t="n">
+      <c r="G9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="12" t="n">
+      <c r="H9" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="H9" s="11" t="n">
+      <c r="I9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="12" t="n">
+      <c r="J9" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="J9" s="13" t="n">
+      <c r="K9" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K9" s="14" t="n">
+      <c r="L9" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="15" t="n">
-        <f aca="false">(B9+D9+F9+H9)*$J$27+(C9+E9+G9+I9)*$J$27+J9*$G$27+K9*$D$27</f>
+      <c r="M9" s="16" t="n">
+        <f aca="false">(C9+E9+G9+I9)*$K$27+(D9+F9+H9+J9)*$K$27+K9*$H$27+L9*$E$27</f>
         <v>439.99</v>
       </c>
-      <c r="M9" s="16" t="n">
-        <f aca="false">L9</f>
+      <c r="N9" s="17" t="n">
+        <f aca="false">M9</f>
         <v>439.99</v>
       </c>
-      <c r="N9" s="0"/>
       <c r="O9" s="0"/>
       <c r="P9" s="0"/>
       <c r="Q9" s="0"/>
@@ -9498,48 +9644,48 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="0"/>
+      <c r="B10" s="11" t="n">
         <v>42646</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="C10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="D10" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="11" t="n">
+      <c r="E10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="12" t="n">
+      <c r="F10" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="11" t="n">
+      <c r="G10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="12" t="n">
+      <c r="H10" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="H10" s="11" t="n">
+      <c r="I10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="12" t="n">
+      <c r="J10" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="J10" s="13" t="n">
+      <c r="K10" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K10" s="14" t="n">
+      <c r="L10" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="15" t="n">
-        <f aca="false">(B10+D10+F10+H10)*$J$27+(C10+E10+G10+I10)*$J$27+J10*$G$27+K10*$D$27</f>
+      <c r="M10" s="16" t="n">
+        <f aca="false">(C10+E10+G10+I10)*$K$27+(D10+F10+H10+J10)*$K$27+K10*$H$27+L10*$E$27</f>
         <v>439.99</v>
       </c>
-      <c r="M10" s="16" t="n">
-        <f aca="false">M9+L10</f>
+      <c r="N10" s="17" t="n">
+        <f aca="false">N9+M10</f>
         <v>879.98</v>
       </c>
-      <c r="N10" s="0"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
       <c r="Q10" s="0"/>
@@ -10552,48 +10698,48 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="0"/>
+      <c r="B11" s="11" t="n">
         <v>42653</v>
       </c>
-      <c r="B11" s="11" t="n">
+      <c r="C11" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="D11" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="11" t="n">
+      <c r="E11" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="12" t="n">
+      <c r="F11" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="11" t="n">
+      <c r="G11" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="12" t="n">
+      <c r="H11" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="11" t="n">
+      <c r="I11" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="12" t="n">
+      <c r="J11" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="J11" s="13" t="n">
+      <c r="K11" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K11" s="14" t="n">
+      <c r="L11" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L11" s="15" t="n">
-        <f aca="false">(B11+D11+F11+H11)*$J$27+(C11+E11+G11+I11)*$J$27+J11*$G$27+K11*$D$27</f>
+      <c r="M11" s="16" t="n">
+        <f aca="false">(C11+E11+G11+I11)*$K$27+(D11+F11+H11+J11)*$K$27+K11*$H$27+L11*$E$27</f>
         <v>439.99</v>
       </c>
-      <c r="M11" s="16" t="n">
-        <f aca="false">M10+L11</f>
+      <c r="N11" s="17" t="n">
+        <f aca="false">N10+M11</f>
         <v>1319.97</v>
       </c>
-      <c r="N11" s="0"/>
       <c r="O11" s="0"/>
       <c r="P11" s="0"/>
       <c r="Q11" s="0"/>
@@ -11606,48 +11752,48 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="0"/>
+      <c r="B12" s="11" t="n">
         <v>42660</v>
       </c>
-      <c r="B12" s="11" t="n">
+      <c r="C12" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="12" t="n">
+      <c r="D12" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D12" s="11" t="n">
+      <c r="E12" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="12" t="n">
+      <c r="F12" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F12" s="11" t="n">
+      <c r="G12" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="12" t="n">
+      <c r="H12" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H12" s="11" t="n">
+      <c r="I12" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="12" t="n">
+      <c r="J12" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J12" s="13" t="n">
+      <c r="K12" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="K12" s="14" t="n">
+      <c r="L12" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L12" s="15" t="n">
-        <f aca="false">(B12+D12+F12+H12)*$J$27+(C12+E12+G12+I12)*$J$27+J12*$G$27+K12*$D$27</f>
+      <c r="M12" s="16" t="n">
+        <f aca="false">(C12+E12+G12+I12)*$K$27+(D12+F12+H12+J12)*$K$27+K12*$H$27+L12*$E$27</f>
         <v>939.98</v>
       </c>
-      <c r="M12" s="16" t="n">
-        <f aca="false">M11+L12</f>
+      <c r="N12" s="17" t="n">
+        <f aca="false">N11+M12</f>
         <v>2259.95</v>
       </c>
-      <c r="N12" s="0"/>
       <c r="O12" s="0"/>
       <c r="P12" s="0"/>
       <c r="Q12" s="0"/>
@@ -12660,48 +12806,48 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="0"/>
+      <c r="B13" s="11" t="n">
         <v>42667</v>
       </c>
-      <c r="B13" s="11" t="n">
+      <c r="C13" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="12" t="n">
+      <c r="D13" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D13" s="11" t="n">
+      <c r="E13" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="12" t="n">
+      <c r="F13" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F13" s="11" t="n">
+      <c r="G13" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="12" t="n">
+      <c r="H13" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H13" s="11" t="n">
+      <c r="I13" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="12" t="n">
+      <c r="J13" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J13" s="13" t="n">
+      <c r="K13" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="K13" s="14" t="n">
+      <c r="L13" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="15" t="n">
-        <f aca="false">(B13+D13+F13+H13)*$J$27+(C13+E13+G13+I13)*$J$27+J13*$G$27+K13*$D$27</f>
+      <c r="M13" s="16" t="n">
+        <f aca="false">(C13+E13+G13+I13)*$K$27+(D13+F13+H13+J13)*$K$27+K13*$H$27+L13*$E$27</f>
         <v>1059.98</v>
       </c>
-      <c r="M13" s="16" t="n">
-        <f aca="false">M12+L13</f>
+      <c r="N13" s="17" t="n">
+        <f aca="false">N12+M13</f>
         <v>3319.93</v>
       </c>
-      <c r="N13" s="0"/>
       <c r="O13" s="0"/>
       <c r="P13" s="0"/>
       <c r="Q13" s="0"/>
@@ -13714,48 +13860,48 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="0"/>
+      <c r="B14" s="11" t="n">
         <v>42674</v>
       </c>
-      <c r="B14" s="11" t="n">
+      <c r="C14" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="12" t="n">
+      <c r="D14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D14" s="11" t="n">
+      <c r="E14" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="12" t="n">
+      <c r="F14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F14" s="11" t="n">
+      <c r="G14" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="12" t="n">
+      <c r="H14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H14" s="11" t="n">
+      <c r="I14" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="12" t="n">
+      <c r="J14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J14" s="13" t="n">
+      <c r="K14" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="K14" s="14" t="n">
+      <c r="L14" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L14" s="15" t="n">
-        <f aca="false">(B14+D14+F14+H14)*$J$27+(C14+E14+G14+I14)*$J$27+J14*$G$27+K14*$D$27</f>
+      <c r="M14" s="16" t="n">
+        <f aca="false">(C14+E14+G14+I14)*$K$27+(D14+F14+H14+J14)*$K$27+K14*$H$27+L14*$E$27</f>
         <v>959.98</v>
       </c>
-      <c r="M14" s="16" t="n">
-        <f aca="false">M13+L14</f>
+      <c r="N14" s="17" t="n">
+        <f aca="false">N13+M14</f>
         <v>4279.91</v>
       </c>
-      <c r="N14" s="0"/>
       <c r="O14" s="0"/>
       <c r="P14" s="0"/>
       <c r="Q14" s="0"/>
@@ -14768,48 +14914,48 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="0"/>
+      <c r="B15" s="11" t="n">
         <v>42681</v>
       </c>
-      <c r="B15" s="11" t="n">
+      <c r="C15" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="12" t="n">
+      <c r="D15" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D15" s="11" t="n">
+      <c r="E15" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="12" t="n">
+      <c r="F15" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="11" t="n">
+      <c r="G15" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="12" t="n">
+      <c r="H15" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H15" s="11" t="n">
+      <c r="I15" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="12" t="n">
+      <c r="J15" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J15" s="13" t="n">
+      <c r="K15" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="K15" s="14" t="n">
+      <c r="L15" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L15" s="15" t="n">
-        <f aca="false">(B15+D15+F15+H15)*$J$27+(C15+E15+G15+I15)*$J$27+J15*$G$27+K15*$D$27</f>
+      <c r="M15" s="16" t="n">
+        <f aca="false">(C15+E15+G15+I15)*$K$27+(D15+F15+H15+J15)*$K$27+K15*$H$27+L15*$E$27</f>
         <v>939.98</v>
       </c>
-      <c r="M15" s="16" t="n">
-        <f aca="false">M14+L15</f>
+      <c r="N15" s="17" t="n">
+        <f aca="false">N14+M15</f>
         <v>5219.89</v>
       </c>
-      <c r="N15" s="0"/>
       <c r="O15" s="0"/>
       <c r="P15" s="0"/>
       <c r="Q15" s="0"/>
@@ -15822,48 +15968,48 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="0"/>
+      <c r="B16" s="11" t="n">
         <v>42688</v>
       </c>
-      <c r="B16" s="11" t="n">
+      <c r="C16" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="12" t="n">
+      <c r="D16" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D16" s="11" t="n">
+      <c r="E16" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="12" t="n">
+      <c r="F16" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F16" s="11" t="n">
+      <c r="G16" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="12" t="n">
+      <c r="H16" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H16" s="11" t="n">
+      <c r="I16" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="12" t="n">
+      <c r="J16" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J16" s="13" t="n">
+      <c r="K16" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="K16" s="14" t="n">
+      <c r="L16" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L16" s="15" t="n">
-        <f aca="false">(B16+D16+F16+H16)*$J$27+(C16+E16+G16+I16)*$J$27+J16*$G$27+K16*$D$27</f>
+      <c r="M16" s="16" t="n">
+        <f aca="false">(C16+E16+G16+I16)*$K$27+(D16+F16+H16+J16)*$K$27+K16*$H$27+L16*$E$27</f>
         <v>939.98</v>
       </c>
-      <c r="M16" s="16" t="n">
-        <f aca="false">M15+L16</f>
+      <c r="N16" s="17" t="n">
+        <f aca="false">N15+M16</f>
         <v>6159.87</v>
       </c>
-      <c r="N16" s="0"/>
       <c r="O16" s="0"/>
       <c r="P16" s="0"/>
       <c r="Q16" s="0"/>
@@ -16876,48 +17022,48 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="0"/>
+      <c r="B17" s="11" t="n">
         <v>42695</v>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="C17" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C17" s="12" t="n">
+      <c r="D17" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="11" t="n">
+      <c r="E17" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="12" t="n">
+      <c r="F17" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F17" s="11" t="n">
+      <c r="G17" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="12" t="n">
+      <c r="H17" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H17" s="11" t="n">
+      <c r="I17" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="12" t="n">
+      <c r="J17" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J17" s="13" t="n">
+      <c r="K17" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="K17" s="14" t="n">
+      <c r="L17" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="15" t="n">
-        <f aca="false">(B17+D17+F17+H17)*$J$27+(C17+E17+G17+I17)*$J$27+J17*$G$27+K17*$D$27</f>
+      <c r="M17" s="16" t="n">
+        <f aca="false">(C17+E17+G17+I17)*$K$27+(D17+F17+H17+J17)*$K$27+K17*$H$27+L17*$E$27</f>
         <v>1059.98</v>
       </c>
-      <c r="M17" s="16" t="n">
-        <f aca="false">M16+L17</f>
+      <c r="N17" s="17" t="n">
+        <f aca="false">N16+M17</f>
         <v>7219.85</v>
       </c>
-      <c r="N17" s="0"/>
       <c r="O17" s="0"/>
       <c r="P17" s="0"/>
       <c r="Q17" s="0"/>
@@ -17930,48 +18076,48 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="n">
+      <c r="A18" s="0"/>
+      <c r="B18" s="11" t="n">
         <v>42702</v>
       </c>
-      <c r="B18" s="11" t="n">
+      <c r="C18" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="12" t="n">
+      <c r="D18" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D18" s="11" t="n">
+      <c r="E18" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E18" s="12" t="n">
+      <c r="F18" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F18" s="11" t="n">
+      <c r="G18" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="12" t="n">
+      <c r="H18" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H18" s="11" t="n">
+      <c r="I18" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="12" t="n">
+      <c r="J18" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J18" s="13" t="n">
+      <c r="K18" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="K18" s="14" t="n">
+      <c r="L18" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L18" s="15" t="n">
-        <f aca="false">(B18+D18+F18+H18)*$J$27+(C18+E18+G18+I18)*$J$27+J18*$G$27+K18*$D$27</f>
+      <c r="M18" s="16" t="n">
+        <f aca="false">(C18+E18+G18+I18)*$K$27+(D18+F18+H18+J18)*$K$27+K18*$H$27+L18*$E$27</f>
         <v>959.98</v>
       </c>
-      <c r="M18" s="16" t="n">
-        <f aca="false">M17+L18</f>
+      <c r="N18" s="17" t="n">
+        <f aca="false">N17+M18</f>
         <v>8179.83</v>
       </c>
-      <c r="N18" s="0"/>
       <c r="O18" s="0"/>
       <c r="P18" s="0"/>
       <c r="Q18" s="0"/>
@@ -18984,48 +19130,48 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="n">
+      <c r="A19" s="0"/>
+      <c r="B19" s="11" t="n">
         <v>42709</v>
       </c>
-      <c r="B19" s="11" t="n">
+      <c r="C19" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="12" t="n">
+      <c r="D19" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="11" t="n">
+      <c r="E19" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="12" t="n">
+      <c r="F19" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F19" s="11" t="n">
+      <c r="G19" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="12" t="n">
+      <c r="H19" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H19" s="11" t="n">
+      <c r="I19" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="12" t="n">
+      <c r="J19" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J19" s="13" t="n">
+      <c r="K19" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="K19" s="14" t="n">
+      <c r="L19" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L19" s="15" t="n">
-        <f aca="false">(B19+D19+F19+H19)*$J$27+(C19+E19+G19+I19)*$J$27+J19*$G$27+K19*$D$27</f>
+      <c r="M19" s="16" t="n">
+        <f aca="false">(C19+E19+G19+I19)*$K$27+(D19+F19+H19+J19)*$K$27+K19*$H$27+L19*$E$27</f>
         <v>939.98</v>
       </c>
-      <c r="M19" s="16" t="n">
-        <f aca="false">M18+L19</f>
+      <c r="N19" s="17" t="n">
+        <f aca="false">N18+M19</f>
         <v>9119.81</v>
       </c>
-      <c r="N19" s="0"/>
       <c r="O19" s="0"/>
       <c r="P19" s="0"/>
       <c r="Q19" s="0"/>
@@ -20038,48 +20184,48 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="n">
+      <c r="A20" s="0"/>
+      <c r="B20" s="11" t="n">
         <v>42716</v>
       </c>
-      <c r="B20" s="11" t="n">
+      <c r="C20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="12" t="n">
+      <c r="D20" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D20" s="11" t="n">
+      <c r="E20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E20" s="12" t="n">
+      <c r="F20" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F20" s="11" t="n">
+      <c r="G20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="12" t="n">
+      <c r="H20" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H20" s="11" t="n">
+      <c r="I20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="12" t="n">
+      <c r="J20" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J20" s="13" t="n">
+      <c r="K20" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="K20" s="14" t="n">
+      <c r="L20" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="L20" s="15" t="n">
-        <f aca="false">(B20+D20+F20+H20)*$J$27+(C20+E20+G20+I20)*$J$27+J20*$G$27+K20*$D$27</f>
+      <c r="M20" s="16" t="n">
+        <f aca="false">(C20+E20+G20+I20)*$K$27+(D20+F20+H20+J20)*$K$27+K20*$H$27+L20*$E$27</f>
         <v>1059.98</v>
       </c>
-      <c r="M20" s="16" t="n">
-        <f aca="false">M19+L20</f>
+      <c r="N20" s="17" t="n">
+        <f aca="false">N19+M20</f>
         <v>10179.79</v>
       </c>
-      <c r="N20" s="0"/>
       <c r="O20" s="0"/>
       <c r="P20" s="0"/>
       <c r="Q20" s="0"/>
@@ -21092,48 +21238,48 @@
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="n">
+      <c r="A21" s="0"/>
+      <c r="B21" s="11" t="n">
         <v>42723</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="C21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="12" t="n">
+      <c r="D21" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="11" t="n">
+      <c r="E21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="12" t="n">
+      <c r="F21" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F21" s="11" t="n">
+      <c r="G21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="12" t="n">
+      <c r="H21" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H21" s="11" t="n">
+      <c r="I21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="12" t="n">
+      <c r="J21" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J21" s="13" t="n">
+      <c r="K21" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="K21" s="14" t="n">
+      <c r="L21" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L21" s="15" t="n">
-        <f aca="false">(B21+D21+F21+H21)*$J$27+(C21+E21+G21+I21)*$J$27+J21*$G$27+K21*$D$27</f>
+      <c r="M21" s="16" t="n">
+        <f aca="false">(C21+E21+G21+I21)*$K$27+(D21+F21+H21+J21)*$K$27+K21*$H$27+L21*$E$27</f>
         <v>959.98</v>
       </c>
-      <c r="M21" s="16" t="n">
-        <f aca="false">M20+L21</f>
+      <c r="N21" s="17" t="n">
+        <f aca="false">N20+M21</f>
         <v>11139.77</v>
       </c>
-      <c r="N21" s="0"/>
       <c r="O21" s="0"/>
       <c r="P21" s="0"/>
       <c r="Q21" s="0"/>
@@ -22146,48 +22292,48 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="n">
+      <c r="A22" s="0"/>
+      <c r="B22" s="11" t="n">
         <v>42730</v>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="C22" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="12" t="n">
+      <c r="D22" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="D22" s="11" t="n">
+      <c r="E22" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="12" t="n">
+      <c r="F22" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="F22" s="11" t="n">
+      <c r="G22" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G22" s="12" t="n">
+      <c r="H22" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="H22" s="11" t="n">
+      <c r="I22" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="12" t="n">
+      <c r="J22" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="J22" s="13" t="n">
+      <c r="K22" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="K22" s="14" t="n">
+      <c r="L22" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L22" s="15" t="n">
-        <f aca="false">(B22+D22+F22+H22)*$J$27+(C22+E22+G22+I22)*$J$27+J22*$G$27+K22*$D$27</f>
+      <c r="M22" s="16" t="n">
+        <f aca="false">(C22+E22+G22+I22)*$K$27+(D22+F22+H22+J22)*$K$27+K22*$H$27+L22*$E$27</f>
         <v>1339.97</v>
       </c>
-      <c r="M22" s="16" t="n">
-        <f aca="false">M21+L22</f>
+      <c r="N22" s="17" t="n">
+        <f aca="false">N21+M22</f>
         <v>12479.74</v>
       </c>
-      <c r="N22" s="0"/>
       <c r="O22" s="0"/>
       <c r="P22" s="0"/>
       <c r="Q22" s="0"/>
@@ -23200,48 +23346,48 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="n">
+      <c r="A23" s="0"/>
+      <c r="B23" s="11" t="n">
         <v>42737</v>
       </c>
-      <c r="B23" s="11" t="n">
+      <c r="C23" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C23" s="12" t="n">
+      <c r="D23" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="D23" s="11" t="n">
+      <c r="E23" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E23" s="12" t="n">
+      <c r="F23" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="F23" s="11" t="n">
+      <c r="G23" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="12" t="n">
+      <c r="H23" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="H23" s="11" t="n">
+      <c r="I23" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I23" s="12" t="n">
+      <c r="J23" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="J23" s="13" t="n">
+      <c r="K23" s="14" t="n">
         <v>16</v>
       </c>
-      <c r="K23" s="14" t="n">
+      <c r="L23" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="L23" s="15" t="n">
-        <f aca="false">(B23+D23+F23+H23)*$J$27+(C23+E23+G23+I23)*$J$27+J23*$G$27+K23*$D$27</f>
+      <c r="M23" s="16" t="n">
+        <f aca="false">(C23+E23+G23+I23)*$K$27+(D23+F23+H23+J23)*$K$27+K23*$H$27+L23*$E$27</f>
         <v>1459.97</v>
       </c>
-      <c r="M23" s="16" t="n">
-        <f aca="false">M22+L23</f>
+      <c r="N23" s="17" t="n">
+        <f aca="false">N22+M23</f>
         <v>13939.71</v>
       </c>
-      <c r="N23" s="0"/>
       <c r="O23" s="0"/>
       <c r="P23" s="0"/>
       <c r="Q23" s="0"/>
@@ -24254,48 +24400,48 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="n">
+      <c r="A24" s="0"/>
+      <c r="B24" s="11" t="n">
         <v>42744</v>
       </c>
-      <c r="B24" s="11" t="n">
+      <c r="C24" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C24" s="12" t="n">
+      <c r="D24" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="D24" s="11" t="n">
+      <c r="E24" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E24" s="12" t="n">
+      <c r="F24" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="F24" s="11" t="n">
+      <c r="G24" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="12" t="n">
+      <c r="H24" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="H24" s="11" t="n">
+      <c r="I24" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="12" t="n">
+      <c r="J24" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="J24" s="13" t="n">
+      <c r="K24" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="K24" s="14" t="n">
+      <c r="L24" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="L24" s="15" t="n">
-        <f aca="false">(B24+D24+F24+H24)*$J$27+(C24+E24+G24+I24)*$J$27+J24*$G$27+K24*$D$27</f>
+      <c r="M24" s="16" t="n">
+        <f aca="false">(C24+E24+G24+I24)*$K$27+(D24+F24+H24+J24)*$K$27+K24*$H$27+L24*$E$27</f>
         <v>1339.97</v>
       </c>
-      <c r="M24" s="16" t="n">
-        <f aca="false">M23+L24</f>
+      <c r="N24" s="17" t="n">
+        <f aca="false">N23+M24</f>
         <v>15279.68</v>
       </c>
-      <c r="N24" s="0"/>
       <c r="O24" s="0"/>
       <c r="P24" s="0"/>
       <c r="Q24" s="0"/>
@@ -25308,55 +25454,55 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="18" t="n">
-        <f aca="false">SUM(B9:B24)</f>
+      <c r="A25" s="0"/>
+      <c r="B25" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="19" t="n">
+        <f aca="false">SUM(C9:C24)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="18" t="n">
-        <f aca="false">SUM(C9:C24)</f>
+      <c r="D25" s="19" t="n">
+        <f aca="false">SUM(D9:D24)</f>
         <v>64</v>
       </c>
-      <c r="D25" s="18" t="n">
-        <f aca="false">SUM(D9:D24)</f>
+      <c r="E25" s="19" t="n">
+        <f aca="false">SUM(E9:E24)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="18" t="n">
-        <f aca="false">SUM(E9:E24)</f>
+      <c r="F25" s="19" t="n">
+        <f aca="false">SUM(F9:F24)</f>
         <v>64</v>
       </c>
-      <c r="F25" s="18" t="n">
-        <f aca="false">SUM(F9:F24)</f>
+      <c r="G25" s="19" t="n">
+        <f aca="false">SUM(G9:G24)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="18" t="n">
-        <f aca="false">SUM(G9:G24)</f>
+      <c r="H25" s="19" t="n">
+        <f aca="false">SUM(H9:H24)</f>
         <v>64</v>
       </c>
-      <c r="H25" s="18" t="n">
-        <f aca="false">SUM(H9:H24)</f>
+      <c r="I25" s="19" t="n">
+        <f aca="false">SUM(I9:I24)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="18" t="n">
-        <f aca="false">SUM(I9:I24)</f>
+      <c r="J25" s="19" t="n">
+        <f aca="false">SUM(J9:J24)</f>
         <v>64</v>
       </c>
-      <c r="J25" s="18" t="n">
-        <f aca="false">SUM(J9:J24)</f>
+      <c r="K25" s="19" t="n">
+        <f aca="false">SUM(K9:K24)</f>
         <v>208</v>
       </c>
-      <c r="K25" s="18" t="n">
-        <f aca="false">SUM(K9:K24)</f>
+      <c r="L25" s="19" t="n">
+        <f aca="false">SUM(L9:L24)</f>
         <v>4</v>
       </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="20" t="n">
-        <f aca="false">M24</f>
+      <c r="M25" s="20"/>
+      <c r="N25" s="21" t="n">
+        <f aca="false">N24</f>
         <v>15279.68</v>
       </c>
-      <c r="N25" s="0"/>
       <c r="O25" s="0"/>
       <c r="P25" s="0"/>
       <c r="Q25" s="0"/>
@@ -27396,29 +27542,29 @@
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="0"/>
+      <c r="C27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22" t="n">
-        <v>100</v>
-      </c>
-      <c r="E27" s="21" t="s">
+      <c r="G27" s="22"/>
+      <c r="H27" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="I27" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22" t="n">
-        <v>10</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="23" t="n">
-        <f aca="false">'Taux horaire d''un technicien'!D15</f>
+      <c r="J27" s="22"/>
+      <c r="K27" s="24" t="n">
+        <f aca="false">'Taux horaire d''un technicien'!E15</f>
         <v>49.99875</v>
       </c>
-      <c r="K27" s="0"/>
       <c r="L27" s="0"/>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -28434,19 +28580,19 @@
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="0"/>
+      <c r="A28" s="0"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
       <c r="N28" s="0"/>
       <c r="O28" s="0"/>
       <c r="P28" s="0"/>
@@ -29460,175 +29606,175 @@
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24"/>
-      <c r="AMJ29" s="2"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
       <c r="B32" s="0"/>
       <c r="C32" s="0"/>
       <c r="D32" s="0"/>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="0"/>
+      <c r="F32" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="24" t="s">
+      <c r="I32" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="27"/>
-      <c r="B33" s="0"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="0"/>
       <c r="D33" s="0"/>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="0"/>
+      <c r="F33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="28" t="n">
+      <c r="G33" s="28" t="n">
         <v>42662</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="H33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="I33" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="24"/>
-      <c r="U33" s="24"/>
-      <c r="V33" s="24"/>
-      <c r="W33" s="24"/>
-      <c r="X33" s="24"/>
-      <c r="Y33" s="24"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:M6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="B5:N6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0" right="0.39375" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -29643,1188 +29789,1188 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="1:33"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="1" sqref="H20 H33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.96356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="3" t="s">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1"/>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2"/>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AMJ1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="AMJ2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="AMJ3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="AMJ4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29" t="s">
+      <c r="J7" s="30"/>
+      <c r="K7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="5" t="s">
+      <c r="L7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="M7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="N7" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="30" t="s">
+      <c r="E8" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="30" t="s">
+      <c r="G8" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="30" t="s">
+      <c r="I8" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="n">
+      <c r="B9" s="33" t="n">
         <v>42639</v>
       </c>
-      <c r="B9" s="33" t="n">
+      <c r="C9" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="34" t="n">
+      <c r="D9" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="33" t="n">
+      <c r="E9" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="34" t="n">
+      <c r="F9" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="33" t="n">
+      <c r="G9" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="34" t="n">
+      <c r="H9" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="H9" s="33" t="n">
+      <c r="I9" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="34" t="n">
+      <c r="J9" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="J9" s="35" t="n">
+      <c r="K9" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="K9" s="36" t="n">
+      <c r="L9" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="37" t="n">
-        <f aca="false">(B9+D9+F9+H9)*$J$27+(C9+E9+G9+I9)*$J$27+J9*$G$27+K9*$D$27</f>
+      <c r="M9" s="38" t="n">
+        <f aca="false">(C9+E9+G9+I9)*$K$27+(D9+F9+H9+J9)*$K$27+K9*$H$27+L9*$E$27</f>
         <v>439.99</v>
       </c>
-      <c r="M9" s="38" t="n">
-        <f aca="false">L9</f>
+      <c r="N9" s="39" t="n">
+        <f aca="false">M9</f>
         <v>439.99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="n">
+      <c r="B10" s="33" t="n">
         <v>42646</v>
       </c>
-      <c r="B10" s="33" t="n">
+      <c r="C10" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="34" t="n">
+      <c r="D10" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="33" t="n">
+      <c r="E10" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="34" t="n">
+      <c r="F10" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="33" t="n">
+      <c r="G10" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="34" t="n">
+      <c r="H10" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="H10" s="33" t="n">
+      <c r="I10" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="34" t="n">
+      <c r="J10" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="J10" s="35" t="n">
+      <c r="K10" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="K10" s="36" t="n">
+      <c r="L10" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="37" t="n">
-        <f aca="false">(B10+D10+F10+H10)*$J$27+(C10+E10+G10+I10)*$J$27+J10*$G$27+K10*$D$27</f>
+      <c r="M10" s="38" t="n">
+        <f aca="false">(C10+E10+G10+I10)*$K$27+(D10+F10+H10+J10)*$K$27+K10*$H$27+L10*$E$27</f>
         <v>439.99</v>
       </c>
-      <c r="M10" s="38" t="n">
-        <f aca="false">M9+L10</f>
+      <c r="N10" s="39" t="n">
+        <f aca="false">N9+M10</f>
         <v>879.98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="n">
+      <c r="B11" s="33" t="n">
         <v>42653</v>
       </c>
-      <c r="B11" s="33" t="n">
+      <c r="C11" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="34" t="n">
+      <c r="D11" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="33" t="n">
+      <c r="E11" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="34" t="n">
+      <c r="F11" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="F11" s="33" t="n">
+      <c r="G11" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="33" t="n">
+      <c r="H11" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="I11" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="34" t="n">
-        <v>2</v>
-      </c>
       <c r="J11" s="35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11" s="36" t="n">
+        <v>5</v>
+      </c>
+      <c r="L11" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="L11" s="37" t="n">
-        <f aca="false">(B11+D11+F11+H11)*$J$27+(C11+E11+G11+I11)*$J$27+J11*$G$27+K11*$D$27</f>
-        <v>439.99</v>
-      </c>
       <c r="M11" s="38" t="n">
-        <f aca="false">M10+L11</f>
-        <v>1319.97</v>
+        <f aca="false">(C11+E11+G11+I11)*$K$27+(D11+F11+H11+J11)*$K$27+K11*$H$27+L11*$E$27</f>
+        <v>549.9875</v>
+      </c>
+      <c r="N11" s="39" t="n">
+        <f aca="false">N10+M11</f>
+        <v>1429.9675</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32" t="n">
+      <c r="B12" s="33" t="n">
         <v>42660</v>
       </c>
-      <c r="B12" s="33" t="n">
+      <c r="C12" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="34" t="n">
+      <c r="D12" s="35" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="D12" s="33" t="n">
+      <c r="G12" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="34" t="n">
+      <c r="H12" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="F12" s="33" t="n">
+      <c r="I12" s="34" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="34" t="n">
+      <c r="J12" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="H12" s="33" t="n">
+      <c r="K12" s="36" t="n">
+        <v>18</v>
+      </c>
+      <c r="L12" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="34" t="n">
-        <v>4</v>
-      </c>
-      <c r="J12" s="35" t="n">
-        <v>14</v>
-      </c>
-      <c r="K12" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="37" t="n">
-        <f aca="false">(B12+D12+F12+H12)*$J$27+(C12+E12+G12+I12)*$J$27+J12*$G$27+K12*$D$27</f>
-        <v>939.98</v>
-      </c>
       <c r="M12" s="38" t="n">
-        <f aca="false">M11+L12</f>
-        <v>2259.95</v>
+        <f aca="false">(C12+E12+G12+I12)*$K$27+(D12+F12+H12+J12)*$K$27+K12*$H$27+L12*$E$27</f>
+        <v>1079.9775</v>
+      </c>
+      <c r="N12" s="39" t="n">
+        <f aca="false">N11+M12</f>
+        <v>2509.945</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="n">
+      <c r="B13" s="40" t="n">
         <v>42667</v>
-      </c>
-      <c r="B13" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B13</f>
-        <v>0</v>
       </c>
       <c r="C13" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C13</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D13</f>
         <v>4</v>
-      </c>
-      <c r="D13" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D13</f>
-        <v>0</v>
       </c>
       <c r="E13" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E13</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F13</f>
         <v>4</v>
-      </c>
-      <c r="F13" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F13</f>
-        <v>0</v>
       </c>
       <c r="G13" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H13</f>
         <v>4</v>
-      </c>
-      <c r="H13" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H13</f>
-        <v>0</v>
       </c>
       <c r="I13" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J13</f>
         <v>4</v>
       </c>
-      <c r="J13" s="42" t="n">
+      <c r="K13" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="K13" s="43" t="n">
+      <c r="L13" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="37" t="n">
-        <f aca="false">(B13+D13+F13+H13)*$J$27+(C13+E13+G13+I13)*$J$27+J13*$G$27+K13*$D$27</f>
+      <c r="M13" s="38" t="n">
+        <f aca="false">(C13+E13+G13+I13)*$K$27+(D13+F13+H13+J13)*$K$27+K13*$H$27+L13*$E$27</f>
         <v>1059.98</v>
       </c>
-      <c r="M13" s="44" t="n">
-        <f aca="false">M12+L13</f>
-        <v>3319.93</v>
+      <c r="N13" s="45" t="n">
+        <f aca="false">N12+M13</f>
+        <v>3569.925</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="n">
+      <c r="B14" s="40" t="n">
         <v>42674</v>
-      </c>
-      <c r="B14" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B14</f>
-        <v>0</v>
       </c>
       <c r="C14" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C14</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D14</f>
         <v>4</v>
-      </c>
-      <c r="D14" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D14</f>
-        <v>0</v>
       </c>
       <c r="E14" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F14</f>
         <v>4</v>
-      </c>
-      <c r="F14" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F14</f>
-        <v>0</v>
       </c>
       <c r="G14" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G14</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H14</f>
         <v>4</v>
-      </c>
-      <c r="H14" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H14</f>
-        <v>0</v>
       </c>
       <c r="I14" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J14</f>
         <v>4</v>
       </c>
-      <c r="J14" s="42" t="n">
+      <c r="K14" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="K14" s="43" t="n">
+      <c r="L14" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L14" s="37" t="n">
-        <f aca="false">(B14+D14+F14+H14)*$J$27+(C14+E14+G14+I14)*$J$27+J14*$G$27+K14*$D$27</f>
+      <c r="M14" s="38" t="n">
+        <f aca="false">(C14+E14+G14+I14)*$K$27+(D14+F14+H14+J14)*$K$27+K14*$H$27+L14*$E$27</f>
         <v>959.98</v>
       </c>
-      <c r="M14" s="44" t="n">
-        <f aca="false">M13+L14</f>
-        <v>4279.91</v>
+      <c r="N14" s="45" t="n">
+        <f aca="false">N13+M14</f>
+        <v>4529.905</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="n">
+      <c r="B15" s="40" t="n">
         <v>42681</v>
-      </c>
-      <c r="B15" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B15</f>
-        <v>0</v>
       </c>
       <c r="C15" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C15</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D15</f>
         <v>4</v>
-      </c>
-      <c r="D15" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D15</f>
-        <v>0</v>
       </c>
       <c r="E15" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E15</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F15</f>
         <v>4</v>
-      </c>
-      <c r="F15" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F15</f>
-        <v>0</v>
       </c>
       <c r="G15" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G15</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H15</f>
         <v>4</v>
-      </c>
-      <c r="H15" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H15</f>
-        <v>0</v>
       </c>
       <c r="I15" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J15</f>
         <v>4</v>
       </c>
-      <c r="J15" s="42" t="n">
+      <c r="K15" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="K15" s="43" t="n">
+      <c r="L15" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L15" s="37" t="n">
-        <f aca="false">(B15+D15+F15+H15)*$J$27+(C15+E15+G15+I15)*$J$27+J15*$G$27+K15*$D$27</f>
+      <c r="M15" s="38" t="n">
+        <f aca="false">(C15+E15+G15+I15)*$K$27+(D15+F15+H15+J15)*$K$27+K15*$H$27+L15*$E$27</f>
         <v>939.98</v>
       </c>
-      <c r="M15" s="44" t="n">
-        <f aca="false">M14+L15</f>
-        <v>5219.89</v>
+      <c r="N15" s="45" t="n">
+        <f aca="false">N14+M15</f>
+        <v>5469.885</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="n">
+      <c r="B16" s="40" t="n">
         <v>42688</v>
-      </c>
-      <c r="B16" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B16</f>
-        <v>0</v>
       </c>
       <c r="C16" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C16</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D16</f>
         <v>4</v>
-      </c>
-      <c r="D16" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D16</f>
-        <v>0</v>
       </c>
       <c r="E16" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E16</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F16</f>
         <v>4</v>
-      </c>
-      <c r="F16" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F16</f>
-        <v>0</v>
       </c>
       <c r="G16" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G16</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H16</f>
         <v>4</v>
-      </c>
-      <c r="H16" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H16</f>
-        <v>0</v>
       </c>
       <c r="I16" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J16</f>
         <v>4</v>
       </c>
-      <c r="J16" s="42" t="n">
+      <c r="K16" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="K16" s="43" t="n">
+      <c r="L16" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L16" s="37" t="n">
-        <f aca="false">(B16+D16+F16+H16)*$J$27+(C16+E16+G16+I16)*$J$27+J16*$G$27+K16*$D$27</f>
+      <c r="M16" s="38" t="n">
+        <f aca="false">(C16+E16+G16+I16)*$K$27+(D16+F16+H16+J16)*$K$27+K16*$H$27+L16*$E$27</f>
         <v>939.98</v>
       </c>
-      <c r="M16" s="44" t="n">
-        <f aca="false">M15+L16</f>
-        <v>6159.87</v>
+      <c r="N16" s="45" t="n">
+        <f aca="false">N15+M16</f>
+        <v>6409.865</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="n">
+      <c r="B17" s="40" t="n">
         <v>42695</v>
-      </c>
-      <c r="B17" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B17</f>
-        <v>0</v>
       </c>
       <c r="C17" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C17</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D17</f>
         <v>4</v>
-      </c>
-      <c r="D17" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D17</f>
-        <v>0</v>
       </c>
       <c r="E17" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F17</f>
         <v>4</v>
-      </c>
-      <c r="F17" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F17</f>
-        <v>0</v>
       </c>
       <c r="G17" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H17</f>
         <v>4</v>
-      </c>
-      <c r="H17" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H17</f>
-        <v>0</v>
       </c>
       <c r="I17" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I17</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J17</f>
         <v>4</v>
       </c>
-      <c r="J17" s="42" t="n">
+      <c r="K17" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="K17" s="43" t="n">
+      <c r="L17" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="37" t="n">
-        <f aca="false">(B17+D17+F17+H17)*$J$27+(C17+E17+G17+I17)*$J$27+J17*$G$27+K17*$D$27</f>
+      <c r="M17" s="38" t="n">
+        <f aca="false">(C17+E17+G17+I17)*$K$27+(D17+F17+H17+J17)*$K$27+K17*$H$27+L17*$E$27</f>
         <v>1059.98</v>
       </c>
-      <c r="M17" s="44" t="n">
-        <f aca="false">M16+L17</f>
-        <v>7219.85</v>
+      <c r="N17" s="45" t="n">
+        <f aca="false">N16+M17</f>
+        <v>7469.845</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="n">
+      <c r="B18" s="40" t="n">
         <v>42702</v>
-      </c>
-      <c r="B18" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B18</f>
-        <v>0</v>
       </c>
       <c r="C18" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C18</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D18</f>
         <v>4</v>
-      </c>
-      <c r="D18" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D18</f>
-        <v>0</v>
       </c>
       <c r="E18" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E18</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F18</f>
         <v>4</v>
-      </c>
-      <c r="F18" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F18</f>
-        <v>0</v>
       </c>
       <c r="G18" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H18</f>
         <v>4</v>
-      </c>
-      <c r="H18" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H18</f>
-        <v>0</v>
       </c>
       <c r="I18" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J18</f>
         <v>4</v>
       </c>
-      <c r="J18" s="42" t="n">
+      <c r="K18" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="K18" s="43" t="n">
+      <c r="L18" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L18" s="37" t="n">
-        <f aca="false">(B18+D18+F18+H18)*$J$27+(C18+E18+G18+I18)*$J$27+J18*$G$27+K18*$D$27</f>
+      <c r="M18" s="38" t="n">
+        <f aca="false">(C18+E18+G18+I18)*$K$27+(D18+F18+H18+J18)*$K$27+K18*$H$27+L18*$E$27</f>
         <v>959.98</v>
       </c>
-      <c r="M18" s="44" t="n">
-        <f aca="false">M17+L18</f>
-        <v>8179.83</v>
+      <c r="N18" s="45" t="n">
+        <f aca="false">N17+M18</f>
+        <v>8429.825</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="n">
+      <c r="B19" s="40" t="n">
         <v>42709</v>
-      </c>
-      <c r="B19" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B19</f>
-        <v>0</v>
       </c>
       <c r="C19" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C19</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D19</f>
         <v>4</v>
-      </c>
-      <c r="D19" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D19</f>
-        <v>0</v>
       </c>
       <c r="E19" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E19</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F19</f>
         <v>4</v>
-      </c>
-      <c r="F19" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F19</f>
-        <v>0</v>
       </c>
       <c r="G19" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G19</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H19</f>
         <v>4</v>
-      </c>
-      <c r="H19" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H19</f>
-        <v>0</v>
       </c>
       <c r="I19" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J19</f>
         <v>4</v>
       </c>
-      <c r="J19" s="42" t="n">
+      <c r="K19" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="K19" s="43" t="n">
+      <c r="L19" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L19" s="37" t="n">
-        <f aca="false">(B19+D19+F19+H19)*$J$27+(C19+E19+G19+I19)*$J$27+J19*$G$27+K19*$D$27</f>
+      <c r="M19" s="38" t="n">
+        <f aca="false">(C19+E19+G19+I19)*$K$27+(D19+F19+H19+J19)*$K$27+K19*$H$27+L19*$E$27</f>
         <v>939.98</v>
       </c>
-      <c r="M19" s="44" t="n">
-        <f aca="false">M18+L19</f>
-        <v>9119.81</v>
+      <c r="N19" s="45" t="n">
+        <f aca="false">N18+M19</f>
+        <v>9369.805</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="n">
+      <c r="B20" s="40" t="n">
         <v>42716</v>
-      </c>
-      <c r="B20" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B20</f>
-        <v>0</v>
       </c>
       <c r="C20" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C20</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D20</f>
         <v>4</v>
-      </c>
-      <c r="D20" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D20</f>
-        <v>0</v>
       </c>
       <c r="E20" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E20</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F20</f>
         <v>4</v>
-      </c>
-      <c r="F20" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F20</f>
-        <v>0</v>
       </c>
       <c r="G20" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G20</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H20</f>
         <v>4</v>
-      </c>
-      <c r="H20" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H20</f>
-        <v>0</v>
       </c>
       <c r="I20" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I20</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J20</f>
         <v>4</v>
       </c>
-      <c r="J20" s="42" t="n">
+      <c r="K20" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="K20" s="43" t="n">
+      <c r="L20" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="L20" s="37" t="n">
-        <f aca="false">(B20+D20+F20+H20)*$J$27+(C20+E20+G20+I20)*$J$27+J20*$G$27+K20*$D$27</f>
+      <c r="M20" s="38" t="n">
+        <f aca="false">(C20+E20+G20+I20)*$K$27+(D20+F20+H20+J20)*$K$27+K20*$H$27+L20*$E$27</f>
         <v>1059.98</v>
       </c>
-      <c r="M20" s="44" t="n">
-        <f aca="false">M19+L20</f>
-        <v>10179.79</v>
+      <c r="N20" s="45" t="n">
+        <f aca="false">N19+M20</f>
+        <v>10429.785</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="n">
+      <c r="B21" s="40" t="n">
         <v>42723</v>
-      </c>
-      <c r="B21" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B21</f>
-        <v>0</v>
       </c>
       <c r="C21" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C21</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D21</f>
         <v>4</v>
-      </c>
-      <c r="D21" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D21</f>
-        <v>0</v>
       </c>
       <c r="E21" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E21</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F21</f>
         <v>4</v>
-      </c>
-      <c r="F21" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F21</f>
-        <v>0</v>
       </c>
       <c r="G21" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H21</f>
         <v>4</v>
-      </c>
-      <c r="H21" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H21</f>
-        <v>0</v>
       </c>
       <c r="I21" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I21</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J21</f>
         <v>4</v>
       </c>
-      <c r="J21" s="42" t="n">
+      <c r="K21" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="K21" s="43" t="n">
+      <c r="L21" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L21" s="37" t="n">
-        <f aca="false">(B21+D21+F21+H21)*$J$27+(C21+E21+G21+I21)*$J$27+J21*$G$27+K21*$D$27</f>
+      <c r="M21" s="38" t="n">
+        <f aca="false">(C21+E21+G21+I21)*$K$27+(D21+F21+H21+J21)*$K$27+K21*$H$27+L21*$E$27</f>
         <v>959.98</v>
       </c>
-      <c r="M21" s="44" t="n">
-        <f aca="false">M20+L21</f>
-        <v>11139.77</v>
+      <c r="N21" s="45" t="n">
+        <f aca="false">N20+M21</f>
+        <v>11389.765</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="n">
+      <c r="B22" s="40" t="n">
         <v>42730</v>
-      </c>
-      <c r="B22" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B22</f>
-        <v>0</v>
       </c>
       <c r="C22" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C22</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D22</f>
         <v>6</v>
-      </c>
-      <c r="D22" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D22</f>
-        <v>0</v>
       </c>
       <c r="E22" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F22</f>
         <v>6</v>
-      </c>
-      <c r="F22" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F22</f>
-        <v>0</v>
       </c>
       <c r="G22" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G22</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H22</f>
         <v>6</v>
-      </c>
-      <c r="H22" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H22</f>
-        <v>0</v>
       </c>
       <c r="I22" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I22</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J22</f>
         <v>6</v>
       </c>
-      <c r="J22" s="42" t="n">
+      <c r="K22" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="K22" s="43" t="n">
+      <c r="L22" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L22" s="37" t="n">
-        <f aca="false">(B22+D22+F22+H22)*$J$27+(C22+E22+G22+I22)*$J$27+J22*$G$27+K22*$D$27</f>
+      <c r="M22" s="38" t="n">
+        <f aca="false">(C22+E22+G22+I22)*$K$27+(D22+F22+H22+J22)*$K$27+K22*$H$27+L22*$E$27</f>
         <v>1339.97</v>
       </c>
-      <c r="M22" s="44" t="n">
-        <f aca="false">M21+L22</f>
-        <v>12479.74</v>
+      <c r="N22" s="45" t="n">
+        <f aca="false">N21+M22</f>
+        <v>12729.735</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="n">
+      <c r="B23" s="40" t="n">
         <v>42737</v>
-      </c>
-      <c r="B23" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B23</f>
-        <v>0</v>
       </c>
       <c r="C23" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C23</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D23</f>
         <v>6</v>
-      </c>
-      <c r="D23" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D23</f>
-        <v>0</v>
       </c>
       <c r="E23" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F23</f>
         <v>6</v>
-      </c>
-      <c r="F23" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F23</f>
-        <v>0</v>
       </c>
       <c r="G23" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G23</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H23</f>
         <v>6</v>
-      </c>
-      <c r="H23" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H23</f>
-        <v>0</v>
       </c>
       <c r="I23" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I23</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J23</f>
         <v>6</v>
       </c>
-      <c r="J23" s="42" t="n">
+      <c r="K23" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="K23" s="43" t="n">
+      <c r="L23" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="L23" s="37" t="n">
-        <f aca="false">(B23+D23+F23+H23)*$J$27+(C23+E23+G23+I23)*$J$27+J23*$G$27+K23*$D$27</f>
+      <c r="M23" s="38" t="n">
+        <f aca="false">(C23+E23+G23+I23)*$K$27+(D23+F23+H23+J23)*$K$27+K23*$H$27+L23*$E$27</f>
         <v>1459.97</v>
       </c>
-      <c r="M23" s="44" t="n">
-        <f aca="false">M22+L23</f>
-        <v>13939.71</v>
+      <c r="N23" s="45" t="n">
+        <f aca="false">N22+M23</f>
+        <v>14189.705</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="n">
+      <c r="B24" s="40" t="n">
         <v>42744</v>
-      </c>
-      <c r="B24" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!B24</f>
-        <v>0</v>
       </c>
       <c r="C24" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!C24</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!D24</f>
         <v>6</v>
-      </c>
-      <c r="D24" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!D24</f>
-        <v>0</v>
       </c>
       <c r="E24" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!F24</f>
         <v>6</v>
-      </c>
-      <c r="F24" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!F24</f>
-        <v>0</v>
       </c>
       <c r="G24" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!G24</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!H24</f>
         <v>6</v>
-      </c>
-      <c r="H24" s="40" t="n">
-        <f aca="false">'Prix de revient initial S3'!H24</f>
-        <v>0</v>
       </c>
       <c r="I24" s="41" t="n">
         <f aca="false">'Prix de revient initial S3'!I24</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="42" t="n">
+        <f aca="false">'Prix de revient initial S3'!J24</f>
         <v>6</v>
       </c>
-      <c r="J24" s="42" t="n">
+      <c r="K24" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="K24" s="43" t="n">
+      <c r="L24" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="L24" s="37" t="n">
-        <f aca="false">(B24+D24+F24+H24)*$J$27+(C24+E24+G24+I24)*$J$27+J24*$G$27+K24*$D$27</f>
+      <c r="M24" s="38" t="n">
+        <f aca="false">(C24+E24+G24+I24)*$K$27+(D24+F24+H24+J24)*$K$27+K24*$H$27+L24*$E$27</f>
         <v>1339.97</v>
       </c>
-      <c r="M24" s="44" t="n">
-        <f aca="false">M23+L24</f>
-        <v>15279.68</v>
+      <c r="N24" s="45" t="n">
+        <f aca="false">N23+M24</f>
+        <v>15529.675</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="17.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="18" t="n">
-        <f aca="false">SUM(B9:B24)</f>
+    <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="19" t="n">
+        <f aca="false">SUM(C9:C24)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="18" t="n">
-        <f aca="false">SUM(C9:C24)</f>
+      <c r="D25" s="19" t="n">
+        <f aca="false">SUM(D9:D24)</f>
+        <v>66</v>
+      </c>
+      <c r="E25" s="19" t="n">
+        <f aca="false">SUM(E9:E24)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="19" t="n">
+        <f aca="false">SUM(F9:F24)</f>
         <v>64</v>
       </c>
-      <c r="D25" s="18" t="n">
-        <f aca="false">SUM(D9:D24)</f>
+      <c r="G25" s="19" t="n">
+        <f aca="false">SUM(G9:G24)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="18" t="n">
-        <f aca="false">SUM(E9:E24)</f>
-        <v>64</v>
-      </c>
-      <c r="F25" s="18" t="n">
-        <f aca="false">SUM(F9:F24)</f>
+      <c r="H25" s="19" t="n">
+        <f aca="false">SUM(H9:H24)</f>
+        <v>65</v>
+      </c>
+      <c r="I25" s="19" t="n">
+        <f aca="false">SUM(I9:I24)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="18" t="n">
-        <f aca="false">SUM(G9:G24)</f>
-        <v>64</v>
-      </c>
-      <c r="H25" s="18" t="n">
-        <f aca="false">SUM(H9:H24)</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="18" t="n">
-        <f aca="false">SUM(I9:I24)</f>
-        <v>64</v>
-      </c>
-      <c r="J25" s="18" t="n">
+      <c r="J25" s="19" t="n">
         <f aca="false">SUM(J9:J24)</f>
-        <v>208</v>
-      </c>
-      <c r="K25" s="18" t="n">
+        <v>65</v>
+      </c>
+      <c r="K25" s="19" t="n">
         <f aca="false">SUM(K9:K24)</f>
+        <v>213</v>
+      </c>
+      <c r="L25" s="19" t="n">
+        <f aca="false">SUM(L9:L24)</f>
         <v>4</v>
       </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="46" t="n">
-        <f aca="false">M24</f>
-        <v>15279.68</v>
+      <c r="M25" s="20"/>
+      <c r="N25" s="47" t="n">
+        <f aca="false">N24</f>
+        <v>15529.675</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMJ26" s="2"/>
+    <row r="26" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="F27" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22" t="n">
-        <v>100</v>
-      </c>
-      <c r="E27" s="21" t="s">
+      <c r="G27" s="22"/>
+      <c r="H27" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="I27" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22" t="n">
-        <v>10</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="23" t="n">
-        <f aca="false">'Taux horaire d''un technicien'!D15</f>
+      <c r="J27" s="22"/>
+      <c r="K27" s="24" t="n">
+        <f aca="false">'Taux horaire d''un technicien'!E15</f>
         <v>49.99875</v>
       </c>
-      <c r="AMJ27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="AMJ28" s="2"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
     </row>
     <row r="29" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24"/>
-      <c r="AMJ29" s="2"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
-      <c r="AMJ30" s="2"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
-      <c r="AMJ31" s="2"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="25" t="s">
+      <c r="A32" s="1"/>
+      <c r="F32" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="24" t="s">
+      <c r="I32" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
-      <c r="AMJ32" s="2"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="24" t="s">
+      <c r="A33" s="1"/>
+      <c r="F33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="28" t="n">
+      <c r="G33" s="28" t="n">
         <v>42662</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="H33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="I33" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="24"/>
-      <c r="U33" s="24"/>
-      <c r="V33" s="24"/>
-      <c r="W33" s="24"/>
-      <c r="X33" s="24"/>
-      <c r="Y33" s="24"/>
-      <c r="AMJ33" s="2"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:M6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="B5:N6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -30842,198 +30988,198 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:Q35"/>
+  <dimension ref="B1:R35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H37" activeCellId="1" sqref="H20 H37"/>
+      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="17" min="9" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.96356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="0" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="48"/>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="49"/>
+      <c r="D6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="I6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="K6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="L6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="M6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="N6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="O6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="P6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="Q6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="R6" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="49" t="s">
+      <c r="C7" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="50" t="n">
+      <c r="D7" s="51" t="n">
         <v>15279.68</v>
       </c>
-      <c r="D7" s="50" t="n">
+      <c r="E7" s="51" t="n">
         <v>15279.68</v>
       </c>
-      <c r="E7" s="50" t="n">
+      <c r="F7" s="51" t="n">
         <v>15279.68</v>
       </c>
-      <c r="F7" s="50" t="n">
+      <c r="G7" s="51" t="n">
         <v>15279.68</v>
       </c>
-      <c r="G7" s="50" t="n">
+      <c r="H7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="50" t="n">
+      <c r="I7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="50" t="n">
+      <c r="J7" s="51" t="n">
         <f aca="false">+[1]'prix de revient à jour'!N24</f>
         <v>0</v>
       </c>
-      <c r="J7" s="50" t="n">
+      <c r="K7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="50" t="n">
+      <c r="L7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="L7" s="50" t="n">
+      <c r="M7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="50" t="n">
+      <c r="N7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="N7" s="50" t="n">
+      <c r="O7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="50" t="n">
+      <c r="P7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="P7" s="50" t="n">
+      <c r="Q7" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" s="50" t="n">
+      <c r="R7" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="51" t="s">
+      <c r="C9" s="29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O28" s="51" t="s">
+      <c r="P28" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="25" t="s">
+      <c r="F34" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="24" t="s">
+      <c r="I34" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="H34" s="25" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="24" t="s">
+      <c r="F35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="28" t="n">
+      <c r="G35" s="28" t="n">
         <v>42662</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="H35" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H35" s="24" t="s">
+      <c r="I35" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -31054,253 +31200,256 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="48" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="48" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="48" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="48" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="48" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="49" width="3.96356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="49" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="49" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="49" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="49" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="49" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="49" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="49" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="3" t="s">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="3"/>
+      <c r="D1" s="0"/>
+      <c r="H1" s="4" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="0"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="0"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="0"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="0"/>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="52" t="s">
+      <c r="B5" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="53"/>
       <c r="C5" s="53"/>
       <c r="D5" s="53"/>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
       <c r="G5" s="53"/>
-      <c r="H5" s="0"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="53"/>
       <c r="B6" s="53"/>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
       <c r="E6" s="53"/>
       <c r="F6" s="53"/>
       <c r="G6" s="53"/>
-      <c r="H6" s="0"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
+      <c r="B7" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="0"/>
-      <c r="D7" s="54" t="n">
+      <c r="D7" s="0"/>
+      <c r="E7" s="54" t="n">
         <v>3000</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="F7" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="0"/>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="C8" s="0"/>
+      <c r="B8" s="0"/>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
+      <c r="B9" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="0"/>
-      <c r="D9" s="54" t="n">
-        <f aca="false">D7+F9*D7</f>
+      <c r="D9" s="0"/>
+      <c r="E9" s="54" t="n">
+        <f aca="false">E7+G9*E7</f>
         <v>4500</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="F9" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="55" t="n">
+      <c r="G9" s="55" t="n">
         <v>0.5</v>
       </c>
-      <c r="G9" s="0"/>
       <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="C10" s="0"/>
+      <c r="B10" s="0"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48" t="s">
+      <c r="B11" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="0"/>
-      <c r="D11" s="54" t="n">
-        <f aca="false">D9+D9*F11</f>
+      <c r="D11" s="0"/>
+      <c r="E11" s="54" t="n">
+        <f aca="false">E9+E9*G11</f>
         <v>5999.85</v>
       </c>
-      <c r="E11" s="0"/>
-      <c r="F11" s="56" t="n">
+      <c r="F11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="56" t="n">
         <v>0.3333</v>
       </c>
-      <c r="G11" s="0"/>
       <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="C12" s="0"/>
+      <c r="B12" s="0"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="48" t="s">
+      <c r="B13" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="0"/>
-      <c r="D13" s="48" t="n">
+      <c r="D13" s="0"/>
+      <c r="E13" s="49" t="n">
         <v>120</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="F13" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="C14" s="0"/>
+      <c r="B14" s="0"/>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="48" t="s">
+      <c r="B15" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="0"/>
-      <c r="D15" s="57" t="n">
-        <f aca="false">D11/D13</f>
+      <c r="D15" s="0"/>
+      <c r="E15" s="57" t="n">
+        <f aca="false">E11/E13</f>
         <v>49.99875</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="F15" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0"/>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0"/>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0"/>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0"/>
       <c r="D19" s="0"/>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="0"/>
+      <c r="F19" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="24" t="s">
+      <c r="I19" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="0"/>
       <c r="D20" s="0"/>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="0"/>
+      <c r="F20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="28" t="n">
+      <c r="G20" s="28" t="n">
         <v>42662</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="H20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="I20" s="4" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour du tableau des coûts
</commit_message>
<xml_diff>
--- a/doc/Gestion des coûts/Gestion des coûts Projet S3.xlsx
+++ b/doc/Gestion des coûts/Gestion des coûts Projet S3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Prix de revient initial S3" sheetId="1" state="visible" r:id="rId2"/>
@@ -196,7 +196,7 @@
     <numFmt numFmtId="174" formatCode="0%"/>
     <numFmt numFmtId="175" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -289,6 +289,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0066CC"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -781,7 +787,7 @@
                   <c:v>15279.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15279.68</c:v>
+                  <c:v>15529.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -821,11 +827,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="18242793"/>
-        <c:axId val="1277854"/>
+        <c:axId val="37905872"/>
+        <c:axId val="12012855"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="18242793"/>
+        <c:axId val="37905872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -862,14 +868,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277854"/>
+        <c:crossAx val="12012855"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1277854"/>
+        <c:axId val="12012855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +919,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18242793"/>
+        <c:crossAx val="37905872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -961,9 +967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>478800</xdr:colOff>
+      <xdr:colOff>478080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -976,8 +982,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18212760" y="0"/>
-          <a:ext cx="1125360" cy="646920"/>
+          <a:off x="14202720" y="0"/>
+          <a:ext cx="791280" cy="646200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -998,9 +1004,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1176120</xdr:colOff>
+      <xdr:colOff>1175400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1013,8 +1019,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1220760" y="0"/>
-          <a:ext cx="1526760" cy="605520"/>
+          <a:off x="1135080" y="0"/>
+          <a:ext cx="1240200" cy="604800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1033,16 +1039,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>2290320</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>223560</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>767880</xdr:colOff>
+      <xdr:colOff>767160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>120960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1055,8 +1061,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19692360" y="360"/>
-          <a:ext cx="1125360" cy="646920"/>
+          <a:off x="15653880" y="360"/>
+          <a:ext cx="543600" cy="646200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1077,9 +1083,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1175760</xdr:colOff>
+      <xdr:colOff>1175040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1092,8 +1098,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1220400" y="0"/>
-          <a:ext cx="1526760" cy="605520"/>
+          <a:off x="1134720" y="0"/>
+          <a:ext cx="1240200" cy="604800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1119,9 +1125,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>272160</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>140760</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1134,8 +1140,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13273200" y="19440"/>
-          <a:ext cx="1086120" cy="646920"/>
+          <a:off x="10177560" y="19440"/>
+          <a:ext cx="859680" cy="646200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1150,15 +1156,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>49320</xdr:colOff>
+      <xdr:colOff>49680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>5040</xdr:colOff>
+      <xdr:colOff>4320</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1166,8 +1172,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1344600" y="1634040"/>
-        <a:ext cx="14547960" cy="2988000"/>
+        <a:off x="1040040" y="1634400"/>
+        <a:ext cx="11327400" cy="2987280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1182,13 +1188,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>357480</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>160560</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>49320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1197,8 +1203,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1652760" y="2214000"/>
-          <a:ext cx="12252240" cy="0"/>
+          <a:off x="1347840" y="2152440"/>
+          <a:ext cx="9318600" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1231,9 +1237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1176840</xdr:colOff>
+      <xdr:colOff>1176120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1246,8 +1252,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="945360" y="0"/>
-          <a:ext cx="1526760" cy="605520"/>
+          <a:off x="859680" y="0"/>
+          <a:ext cx="1306800" cy="604800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1257,6 +1263,76 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>576000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>140760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>403560</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>72000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="842400" y="2068560"/>
+          <a:ext cx="551520" cy="281520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="0066cc"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>15 279,68</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1273,13 +1349,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>43560</xdr:colOff>
+      <xdr:colOff>42840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 1" descr=""/>
+        <xdr:cNvPr id="9" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1288,8 +1364,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13475160" y="19800"/>
-          <a:ext cx="1084320" cy="646920"/>
+          <a:off x="10369800" y="19800"/>
+          <a:ext cx="807480" cy="646200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1310,13 +1386,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 2" descr=""/>
+        <xdr:cNvPr id="10" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1325,8 +1401,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1618920" y="0"/>
-          <a:ext cx="1526760" cy="605520"/>
+          <a:off x="1342800" y="0"/>
+          <a:ext cx="1116360" cy="604800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1354,19 +1430,19 @@
   </sheetPr>
   <dimension ref="1:33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.96356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="2" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="2" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="3.8582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="2" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="2" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="2" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29791,20 +29867,20 @@
   </sheetPr>
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.96356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.8582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30991,21 +31067,21 @@
   <dimension ref="B1:R35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.96356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="14" min="10" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.8582995951417"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="10" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31108,7 +31184,7 @@
         <v>15279.68</v>
       </c>
       <c r="G7" s="51" t="n">
-        <v>15279.68</v>
+        <v>15529.68</v>
       </c>
       <c r="H7" s="51" t="n">
         <v>0</v>
@@ -31202,22 +31278,22 @@
   </sheetPr>
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="49" width="3.96356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="49" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="49" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="49" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="49" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="49" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="49" width="3.8582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="49" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="49" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="49" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="49" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="49" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="49" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="49" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="49" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="49" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="49" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>